<commit_message>
update bảng yêu cầu
</commit_message>
<xml_diff>
--- a/Phân tích/Yêu cầu/Yêu cầu an toàn.xlsx
+++ b/Phân tích/Yêu cầu/Yêu cầu an toàn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auhai\Documents\GitHub\CNPM\Phân tích\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Phân tích\Yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBE686EE-E053-48CB-93D3-B6B5FE775E8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2C3571-C7A5-4B89-B63F-625A5EFCAD4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{F4D7E051-BBF1-4EAE-A46A-EA71EEC8B095}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F4D7E051-BBF1-4EAE-A46A-EA71EEC8B095}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>Phần mềm</t>
   </si>
   <si>
-    <t>Cho biết hồ sợ nhân viên, khách hàng, đơn đặt hàng, hoá đơn bán hàng cần phục hồi</t>
-  </si>
-  <si>
-    <t>Cho biết hồ sợ nhân viên, khách hàng, đơn đặt hàng, hoá đơn bán hàng cần huỷ</t>
-  </si>
-  <si>
     <t>Huỷ thật sự</t>
   </si>
   <si>
@@ -76,13 +70,19 @@
   </si>
   <si>
     <t>Yêu cầu an toàn</t>
+  </si>
+  <si>
+    <t>Cho biết hồ sơ nhân viên, khách hàng, đơn đặt hàng, hoá đơn bán hàng cần phục hồi</t>
+  </si>
+  <si>
+    <t>Cho biết hồ sơ nhân viên, khách hàng, đơn đặt hàng, hoá đơn bán hàng cần huỷ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,11 @@
       <color theme="1"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,32 +118,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,35 +483,40 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="62.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="75.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="5.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="92" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="F1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,273 +545,182 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="F3" s="3">
+      <c r="D3" s="4"/>
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="3"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>